<commit_message>
adding materials from template
</commit_message>
<xml_diff>
--- a/template_example.xlsx
+++ b/template_example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAD5BEB4-50B8-4F7B-9560-6B03200B3185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2EF2BBD-CA6C-4907-8366-A9E2CA033CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Talep No</t>
+    <t>MaterialID</t>
   </si>
   <si>
-    <t>Miktar</t>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -95,8 +95,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{43A08C96-7614-4181-9926-F71069754623}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3" xr:uid="{43A08C96-7614-4181-9926-F71069754623}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B94BB901-5748-4DF5-AFC6-B8DD8A5C1A55}" name="Talep No"/>
-    <tableColumn id="2" xr3:uid="{E8450F1A-F487-4FBB-8B57-54EBB9F8FA80}" name="Miktar"/>
+    <tableColumn id="1" xr3:uid="{B94BB901-5748-4DF5-AFC6-B8DD8A5C1A55}" name="MaterialID"/>
+    <tableColumn id="2" xr3:uid="{E8450F1A-F487-4FBB-8B57-54EBB9F8FA80}" name="Quantity"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>